<commit_message>
Compiling spreadsheets for 2021-02 synoptic
</commit_message>
<xml_diff>
--- a/Synoptic/Data/2021-02/202102_GHGs_Key.xlsx
+++ b/Synoptic/Data/2021-02/202102_GHGs_Key.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carla López Lloreda\Dropbox\Grad school\Research\Delmarva project\Data\GC\Synoptic\2021-02\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carla López Lloreda\Dropbox\Grad school\Research\Delmarva project\Data\Synoptic\Data\2021-02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{695276B2-A17D-4D54-864B-F37FA47D9B44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2266CF1A-E567-4303-9681-4D7A034F44A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{38FA2F06-98F9-484C-9E5A-9DDA4CAAD6BC}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="185">
   <si>
     <t>AG-SW</t>
   </si>
@@ -71,9 +71,6 @@
   </si>
   <si>
     <t>FN-SW</t>
-  </si>
-  <si>
-    <t>FR-SW</t>
   </si>
   <si>
     <t>JA-SW</t>
@@ -979,10 +976,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C81E5CE-91BB-4950-9A9B-B51DE114D908}">
-  <dimension ref="A1:M123"/>
+  <dimension ref="A1:M121"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G119" sqref="G119"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1001,43 +998,43 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="G1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="I1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -1054,23 +1051,23 @@
         <v>20210225</v>
       </c>
       <c r="E2" t="str">
-        <f t="shared" ref="E2:E33" si="0">_xlfn.CONCAT(A2,"-",B2,"-",C2,"-",D2)</f>
+        <f>_xlfn.CONCAT(A2,"-",B2,"-",C2,"-",D2)</f>
         <v>AG-SW-GHG-R1-20210225</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I2" s="3">
         <v>5.7</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L2">
         <v>0</v>
       </c>
       <c r="M2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -1081,29 +1078,29 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3">
         <v>20210225</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(A3,"-",B3,"-",C3,"-",D3)</f>
         <v>AG-SW-GHG-R2-20210225</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I3" s="3">
         <v>5.7</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
       <c r="M3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -1114,34 +1111,34 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D4">
         <v>20210225</v>
       </c>
       <c r="E4" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(A4,"-",B4,"-",C4,"-",D4)</f>
         <v>AG-SW-GHG-R3-20210225</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I4" s="3">
         <v>5.7</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L4">
         <v>0</v>
       </c>
       <c r="M4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>63</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -1153,94 +1150,94 @@
         <v>20210224</v>
       </c>
       <c r="E5" t="str">
-        <f t="shared" si="0"/>
-        <v>BD-CH-GHG-R1-20210224</v>
+        <f>_xlfn.CONCAT(A5,"-",B5,"-",C5,"-",D5)</f>
+        <v>BD-SW-GHG-R1-20210224</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="I5" s="3">
-        <v>10.199999999999999</v>
+        <v>4.5</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M5" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>63</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D6">
         <v>20210224</v>
       </c>
       <c r="E6" t="str">
-        <f t="shared" si="0"/>
-        <v>BD-CH-GHG-R2-20210224</v>
+        <f>_xlfn.CONCAT(A6,"-",B6,"-",C6,"-",D6)</f>
+        <v>BD-SW-GHG-R2-20210224</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I6" s="3">
-        <v>10.199999999999999</v>
+        <v>4.5</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M6" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>63</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7">
         <v>20210224</v>
       </c>
       <c r="E7" t="str">
-        <f t="shared" si="0"/>
-        <v>BD-CH-GHG-R3-20210224</v>
+        <f>_xlfn.CONCAT(A7,"-",B7,"-",C7,"-",D7)</f>
+        <v>BD-SW-GHG-R3-20210224</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I7" s="3">
-        <v>10.199999999999999</v>
+        <v>4.5</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M7" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>3</v>
+        <v>62</v>
       </c>
       <c r="B8" t="s">
         <v>1</v>
@@ -1252,89 +1249,89 @@
         <v>20210224</v>
       </c>
       <c r="E8" t="str">
-        <f t="shared" si="0"/>
-        <v>BD-SW-GHG-R1-20210224</v>
+        <f>_xlfn.CONCAT(A8,"-",B8,"-",C8,"-",D8)</f>
+        <v>BD-CH-GHG-R1-20210224</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="I8" s="3">
-        <v>4.5</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M8" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>3</v>
+        <v>62</v>
       </c>
       <c r="B9" t="s">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D9">
         <v>20210224</v>
       </c>
       <c r="E9" t="str">
-        <f t="shared" si="0"/>
-        <v>BD-SW-GHG-R2-20210224</v>
+        <f>_xlfn.CONCAT(A9,"-",B9,"-",C9,"-",D9)</f>
+        <v>BD-CH-GHG-R2-20210224</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="I9" s="3">
-        <v>4.5</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M9" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>3</v>
+        <v>62</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D10">
         <v>20210224</v>
       </c>
       <c r="E10" t="str">
-        <f t="shared" si="0"/>
-        <v>BD-SW-GHG-R3-20210224</v>
+        <f>_xlfn.CONCAT(A10,"-",B10,"-",C10,"-",D10)</f>
+        <v>BD-CH-GHG-R3-20210224</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="I10" s="3">
-        <v>4.5</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M10" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
@@ -1351,23 +1348,23 @@
         <v>20210225</v>
       </c>
       <c r="E11" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(A11,"-",B11,"-",C11,"-",D11)</f>
         <v>CR-SW-GHG-R1-20210225</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I11" s="3">
         <v>7.8</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L11">
         <v>0</v>
       </c>
       <c r="M11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
@@ -1378,29 +1375,29 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D12">
         <v>20210225</v>
       </c>
       <c r="E12" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(A12,"-",B12,"-",C12,"-",D12)</f>
         <v>CR-SW-GHG-R2-20210225</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I12" s="3">
         <v>7.8</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L12">
         <v>0</v>
       </c>
       <c r="M12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
@@ -1411,29 +1408,29 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D13">
         <v>20210225</v>
       </c>
       <c r="E13" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(A13,"-",B13,"-",C13,"-",D13)</f>
         <v>CR-SW-GHG-R3-20210225</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I13" s="3">
         <v>7.8</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L13">
         <v>0</v>
       </c>
       <c r="M13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
@@ -1450,23 +1447,23 @@
         <v>20210225</v>
       </c>
       <c r="E14" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(A14,"-",B14,"-",C14,"-",D14)</f>
         <v>DB-SW-GHG-R1-20210225</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I14" s="3">
         <v>5.4</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L14">
         <v>0</v>
       </c>
       <c r="M14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
@@ -1477,29 +1474,29 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D15">
         <v>20210225</v>
       </c>
       <c r="E15" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(A15,"-",B15,"-",C15,"-",D15)</f>
         <v>DB-SW-GHG-R2-20210225</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I15" s="3">
         <v>5.4</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L15">
         <v>0</v>
       </c>
       <c r="M15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
@@ -1510,29 +1507,29 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D16">
         <v>20210225</v>
       </c>
       <c r="E16" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(A16,"-",B16,"-",C16,"-",D16)</f>
         <v>DB-SW-GHG-R3-20210225</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I16" s="3">
         <v>5.4</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L16">
         <v>0</v>
       </c>
       <c r="M16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
@@ -1549,23 +1546,23 @@
         <v>20210225</v>
       </c>
       <c r="E17" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(A17,"-",B17,"-",C17,"-",D17)</f>
         <v>DB-UW1-GHG-R1-20210225</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I17" s="3">
         <v>6.9</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L17">
         <v>0</v>
       </c>
       <c r="M17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
@@ -1576,29 +1573,29 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D18">
         <v>20210225</v>
       </c>
       <c r="E18" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(A18,"-",B18,"-",C18,"-",D18)</f>
         <v>DB-UW1-GHG-R2-20210225</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I18" s="3">
         <v>6.9</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L18">
         <v>0</v>
       </c>
       <c r="M18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
@@ -1609,29 +1606,29 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D19">
         <v>20210225</v>
       </c>
       <c r="E19" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(A19,"-",B19,"-",C19,"-",D19)</f>
         <v>DB-UW1-GHG-R3-20210225</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I19" s="3">
         <v>6.9</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L19">
         <v>0</v>
       </c>
       <c r="M19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
@@ -1648,23 +1645,23 @@
         <v>20210226</v>
       </c>
       <c r="E20" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(A20,"-",B20,"-",C20,"-",D20)</f>
         <v>DF-SW-GHG-R1-20210226</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I20" s="3">
         <v>7.9</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L20">
         <v>0</v>
       </c>
       <c r="M20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
@@ -1675,29 +1672,29 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D21">
         <v>20210226</v>
       </c>
       <c r="E21" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(A21,"-",B21,"-",C21,"-",D21)</f>
         <v>DF-SW-GHG-R2-20210226</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I21" s="3">
         <v>7.9</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L21">
         <v>0</v>
       </c>
       <c r="M21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
@@ -1708,34 +1705,34 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D22">
         <v>20210226</v>
       </c>
       <c r="E22" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(A22,"-",B22,"-",C22,"-",D22)</f>
         <v>DF-SW-GHG-R3-20210226</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I22" s="3">
         <v>7.9</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L22">
         <v>0</v>
       </c>
       <c r="M22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>64</v>
+        <v>8</v>
       </c>
       <c r="B23" t="s">
         <v>1</v>
@@ -1747,103 +1744,94 @@
         <v>20210224</v>
       </c>
       <c r="E23" t="str">
-        <f t="shared" si="0"/>
-        <v>DK-CH-GHG-R1-20210224</v>
+        <f>_xlfn.CONCAT(A23,"-",B23,"-",C23,"-",D23)</f>
+        <v>DK-SW-GHG-R1-20210224</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>61</v>
+        <v>101</v>
+      </c>
+      <c r="I23" s="3">
+        <v>5.7</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="K23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="L23">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M23" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>64</v>
+        <v>8</v>
       </c>
       <c r="B24" t="s">
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D24">
         <v>20210224</v>
       </c>
       <c r="E24" t="str">
-        <f t="shared" si="0"/>
-        <v>DK-CH-GHG-R2-20210224</v>
+        <f>_xlfn.CONCAT(A24,"-",B24,"-",C24,"-",D24)</f>
+        <v>DK-SW-GHG-R2-20210224</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>61</v>
+        <v>102</v>
+      </c>
+      <c r="I24" s="3">
+        <v>5.7</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="K24" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="L24">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M24" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>64</v>
+        <v>8</v>
       </c>
       <c r="B25" t="s">
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D25">
         <v>20210224</v>
       </c>
       <c r="E25" t="str">
-        <f t="shared" si="0"/>
-        <v>DK-CH-GHG-R3-20210224</v>
+        <f>_xlfn.CONCAT(A25,"-",B25,"-",C25,"-",D25)</f>
+        <v>DK-SW-GHG-R3-20210224</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>61</v>
+        <v>103</v>
+      </c>
+      <c r="I25" s="3">
+        <v>5.7</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="K25" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="L25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M25" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>8</v>
+        <v>63</v>
       </c>
       <c r="B26" t="s">
         <v>1</v>
@@ -1855,89 +1843,98 @@
         <v>20210224</v>
       </c>
       <c r="E26" t="str">
-        <f t="shared" si="0"/>
-        <v>DK-SW-GHG-R1-20210224</v>
+        <f>_xlfn.CONCAT(A26,"-",B26,"-",C26,"-",D26)</f>
+        <v>DK-CH-GHG-R1-20210224</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="I26" s="3">
-        <v>5.7</v>
+        <v>98</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
+      </c>
+      <c r="K26" t="s">
+        <v>60</v>
       </c>
       <c r="L26">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M26" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>8</v>
+        <v>63</v>
       </c>
       <c r="B27" t="s">
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D27">
         <v>20210224</v>
       </c>
       <c r="E27" t="str">
-        <f t="shared" si="0"/>
-        <v>DK-SW-GHG-R2-20210224</v>
+        <f>_xlfn.CONCAT(A27,"-",B27,"-",C27,"-",D27)</f>
+        <v>DK-CH-GHG-R2-20210224</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="I27" s="3">
-        <v>5.7</v>
+        <v>99</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
+      </c>
+      <c r="K27" t="s">
+        <v>60</v>
       </c>
       <c r="L27">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M27" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>8</v>
+        <v>63</v>
       </c>
       <c r="B28" t="s">
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D28">
         <v>20210224</v>
       </c>
       <c r="E28" t="str">
-        <f t="shared" si="0"/>
-        <v>DK-SW-GHG-R3-20210224</v>
+        <f>_xlfn.CONCAT(A28,"-",B28,"-",C28,"-",D28)</f>
+        <v>DK-CH-GHG-R3-20210224</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="I28" s="3">
-        <v>5.7</v>
+        <v>100</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
+      </c>
+      <c r="K28" t="s">
+        <v>60</v>
       </c>
       <c r="L28">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M28" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
@@ -1954,23 +1951,23 @@
         <v>20210224</v>
       </c>
       <c r="E29" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(A29,"-",B29,"-",C29,"-",D29)</f>
         <v>DK-UW1-GHG-R1-20210224</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I29" s="3">
         <v>12.1</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L29">
         <v>0</v>
       </c>
       <c r="M29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
@@ -1981,29 +1978,29 @@
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D30">
         <v>20210224</v>
       </c>
       <c r="E30" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(A30,"-",B30,"-",C30,"-",D30)</f>
         <v>DK-UW1-GHG-R2-20210224</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I30" s="3">
         <v>12.1</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L30">
         <v>0</v>
       </c>
       <c r="M30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
@@ -2014,29 +2011,29 @@
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D31">
         <v>20210224</v>
       </c>
       <c r="E31" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(A31,"-",B31,"-",C31,"-",D31)</f>
         <v>DK-UW1-GHG-R3-20210224</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I31" s="3">
         <v>12.1</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L31">
         <v>0</v>
       </c>
       <c r="M31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
@@ -2053,23 +2050,23 @@
         <v>20210224</v>
       </c>
       <c r="E32" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(A32,"-",B32,"-",C32,"-",D32)</f>
         <v>DK-UW2-GHG-R1-20210224</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I32" s="3">
         <v>9.8000000000000007</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L32">
         <v>0</v>
       </c>
       <c r="M32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
@@ -2080,29 +2077,29 @@
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D33">
         <v>20210224</v>
       </c>
       <c r="E33" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(A33,"-",B33,"-",C33,"-",D33)</f>
         <v>DK-UW2-GHG-R2-20210224</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I33" s="3">
         <v>9.8000000000000007</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L33">
         <v>0</v>
       </c>
       <c r="M33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
@@ -2113,29 +2110,29 @@
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D34">
         <v>20210224</v>
       </c>
       <c r="E34" t="str">
-        <f t="shared" ref="E34:E65" si="1">_xlfn.CONCAT(A34,"-",B34,"-",C34,"-",D34)</f>
+        <f>_xlfn.CONCAT(A34,"-",B34,"-",C34,"-",D34)</f>
         <v>DK-UW2-GHG-R3-20210224</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I34" s="3">
         <v>9.8000000000000007</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L34">
         <v>0</v>
       </c>
       <c r="M34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
@@ -2152,23 +2149,23 @@
         <v>20210225</v>
       </c>
       <c r="E35" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(A35,"-",B35,"-",C35,"-",D35)</f>
         <v>FN-SW-GHG-R1-20210225</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I35" s="3">
         <v>8.3000000000000007</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L35">
         <v>0</v>
       </c>
       <c r="M35" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
@@ -2179,29 +2176,29 @@
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D36">
         <v>20210225</v>
       </c>
       <c r="E36" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(A36,"-",B36,"-",C36,"-",D36)</f>
         <v>FN-SW-GHG-R2-20210225</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I36" s="3">
         <v>8.3000000000000007</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L36">
         <v>0</v>
       </c>
       <c r="M36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
@@ -2212,29 +2209,29 @@
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D37">
         <v>20210225</v>
       </c>
       <c r="E37" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(A37,"-",B37,"-",C37,"-",D37)</f>
         <v>FN-SW-GHG-R3-20210225</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I37" s="3">
         <v>8.3000000000000007</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L37">
         <v>0</v>
       </c>
       <c r="M37" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">
@@ -2248,24 +2245,26 @@
         <v>2</v>
       </c>
       <c r="D38">
-        <v>20210224</v>
+        <v>20210226</v>
       </c>
       <c r="E38" t="str">
-        <f t="shared" si="1"/>
-        <v>FR-SW-GHG-R1-20210224</v>
-      </c>
-      <c r="F38" s="6"/>
+        <f>_xlfn.CONCAT(A38,"-",B38,"-",C38,"-",D38)</f>
+        <v>JA-SW-GHG-R1-20210226</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>113</v>
+      </c>
       <c r="I38" s="3">
-        <v>8.1</v>
+        <v>5</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="L38">
         <v>0</v>
       </c>
       <c r="M38" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
@@ -2276,27 +2275,29 @@
         <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D39">
-        <v>20210224</v>
+        <v>20210226</v>
       </c>
       <c r="E39" t="str">
-        <f t="shared" si="1"/>
-        <v>FR-SW-GHG-R2-20210224</v>
-      </c>
-      <c r="F39" s="6"/>
+        <f>_xlfn.CONCAT(A39,"-",B39,"-",C39,"-",D39)</f>
+        <v>JA-SW-GHG-R2-20210226</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>114</v>
+      </c>
       <c r="I39" s="3">
-        <v>8.1</v>
+        <v>5</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="L39">
         <v>0</v>
       </c>
       <c r="M39" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
@@ -2307,27 +2308,29 @@
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D40">
-        <v>20210224</v>
+        <v>20210226</v>
       </c>
       <c r="E40" t="str">
-        <f t="shared" si="1"/>
-        <v>FR-SW-GHG-R3-20210224</v>
-      </c>
-      <c r="F40" s="6"/>
+        <f>_xlfn.CONCAT(A40,"-",B40,"-",C40,"-",D40)</f>
+        <v>JA-SW-GHG-R3-20210226</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>115</v>
+      </c>
       <c r="I40" s="3">
-        <v>8.1</v>
+        <v>5</v>
       </c>
       <c r="J40" s="3" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="L40">
         <v>0</v>
       </c>
       <c r="M40" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.3">
@@ -2344,23 +2347,23 @@
         <v>20210226</v>
       </c>
       <c r="E41" t="str">
-        <f t="shared" si="1"/>
-        <v>JA-SW-GHG-R1-20210226</v>
+        <f>_xlfn.CONCAT(A41,"-",B41,"-",C41,"-",D41)</f>
+        <v>JB-SW-GHG-R1-20210226</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I41" s="3">
-        <v>5</v>
+        <v>5.6</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L41">
         <v>0</v>
       </c>
       <c r="M41" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
@@ -2371,29 +2374,29 @@
         <v>1</v>
       </c>
       <c r="C42" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D42">
         <v>20210226</v>
       </c>
       <c r="E42" t="str">
-        <f t="shared" si="1"/>
-        <v>JA-SW-GHG-R2-20210226</v>
+        <f>_xlfn.CONCAT(A42,"-",B42,"-",C42,"-",D42)</f>
+        <v>JB-SW-GHG-R2-20210226</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="I42" s="3">
-        <v>5</v>
+        <v>5.6</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L42">
         <v>0</v>
       </c>
       <c r="M42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.3">
@@ -2404,29 +2407,29 @@
         <v>1</v>
       </c>
       <c r="C43" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D43">
         <v>20210226</v>
       </c>
       <c r="E43" t="str">
-        <f t="shared" si="1"/>
-        <v>JA-SW-GHG-R3-20210226</v>
+        <f>_xlfn.CONCAT(A43,"-",B43,"-",C43,"-",D43)</f>
+        <v>JB-SW-GHG-R3-20210226</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="I43" s="3">
-        <v>5</v>
+        <v>5.6</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L43">
         <v>0</v>
       </c>
       <c r="M43" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.3">
@@ -2443,23 +2446,23 @@
         <v>20210226</v>
       </c>
       <c r="E44" t="str">
-        <f t="shared" si="1"/>
-        <v>JB-SW-GHG-R1-20210226</v>
+        <f>_xlfn.CONCAT(A44,"-",B44,"-",C44,"-",D44)</f>
+        <v>JB-UW1-GHG-R1-20210226</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="I44" s="3">
-        <v>5.6</v>
+        <v>6.1</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L44">
         <v>0</v>
       </c>
       <c r="M44" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.3">
@@ -2470,29 +2473,29 @@
         <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D45">
         <v>20210226</v>
       </c>
       <c r="E45" t="str">
-        <f t="shared" si="1"/>
-        <v>JB-SW-GHG-R2-20210226</v>
+        <f>_xlfn.CONCAT(A45,"-",B45,"-",C45,"-",D45)</f>
+        <v>JB-UW1-GHG-R2-20210226</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="I45" s="3">
-        <v>5.6</v>
+        <v>6.1</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L45">
         <v>0</v>
       </c>
       <c r="M45" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.3">
@@ -2503,29 +2506,29 @@
         <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D46">
         <v>20210226</v>
       </c>
       <c r="E46" t="str">
-        <f t="shared" si="1"/>
-        <v>JB-SW-GHG-R3-20210226</v>
+        <f>_xlfn.CONCAT(A46,"-",B46,"-",C46,"-",D46)</f>
+        <v>JB-UW1-GHG-R3-20210226</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="I46" s="3">
-        <v>5.6</v>
+        <v>6.1</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L46">
         <v>0</v>
       </c>
       <c r="M46" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.3">
@@ -2542,23 +2545,23 @@
         <v>20210226</v>
       </c>
       <c r="E47" t="str">
-        <f t="shared" si="1"/>
-        <v>JB-UW1-GHG-R1-20210226</v>
+        <f>_xlfn.CONCAT(A47,"-",B47,"-",C47,"-",D47)</f>
+        <v>JB-UW2-GHG-R1-20210226</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="I47" s="3">
-        <v>6.1</v>
+        <v>6.7</v>
       </c>
       <c r="J47" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L47">
         <v>0</v>
       </c>
       <c r="M47" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.3">
@@ -2569,29 +2572,29 @@
         <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D48">
         <v>20210226</v>
       </c>
       <c r="E48" t="str">
-        <f t="shared" si="1"/>
-        <v>JB-UW1-GHG-R2-20210226</v>
+        <f>_xlfn.CONCAT(A48,"-",B48,"-",C48,"-",D48)</f>
+        <v>JB-UW2-GHG-R2-20210226</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="I48" s="3">
-        <v>6.1</v>
+        <v>6.7</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L48">
         <v>0</v>
       </c>
       <c r="M48" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.3">
@@ -2602,29 +2605,29 @@
         <v>1</v>
       </c>
       <c r="C49" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D49">
         <v>20210226</v>
       </c>
       <c r="E49" t="str">
-        <f t="shared" si="1"/>
-        <v>JB-UW1-GHG-R3-20210226</v>
+        <f>_xlfn.CONCAT(A49,"-",B49,"-",C49,"-",D49)</f>
+        <v>JB-UW2-GHG-R3-20210226</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="I49" s="3">
-        <v>6.1</v>
+        <v>6.7</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L49">
         <v>0</v>
       </c>
       <c r="M49" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.3">
@@ -2641,23 +2644,23 @@
         <v>20210226</v>
       </c>
       <c r="E50" t="str">
-        <f t="shared" si="1"/>
-        <v>JB-UW2-GHG-R1-20210226</v>
+        <f>_xlfn.CONCAT(A50,"-",B50,"-",C50,"-",D50)</f>
+        <v>JC-SW-GHG-R1-20210226</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="I50" s="3">
-        <v>6.7</v>
+        <v>5.4</v>
       </c>
       <c r="J50" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L50">
         <v>0</v>
       </c>
       <c r="M50" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.3">
@@ -2668,29 +2671,29 @@
         <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D51">
         <v>20210226</v>
       </c>
       <c r="E51" t="str">
-        <f t="shared" si="1"/>
-        <v>JB-UW2-GHG-R2-20210226</v>
+        <f>_xlfn.CONCAT(A51,"-",B51,"-",C51,"-",D51)</f>
+        <v>JC-SW-GHG-R2-20210226</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="I51" s="3">
-        <v>6.7</v>
+        <v>5.4</v>
       </c>
       <c r="J51" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L51">
         <v>0</v>
       </c>
       <c r="M51" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.3">
@@ -2701,29 +2704,29 @@
         <v>1</v>
       </c>
       <c r="C52" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D52">
         <v>20210226</v>
       </c>
       <c r="E52" t="str">
-        <f t="shared" si="1"/>
-        <v>JB-UW2-GHG-R3-20210226</v>
+        <f>_xlfn.CONCAT(A52,"-",B52,"-",C52,"-",D52)</f>
+        <v>JC-SW-GHG-R3-20210226</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="I52" s="3">
-        <v>6.7</v>
+        <v>5.4</v>
       </c>
       <c r="J52" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L52">
         <v>0</v>
       </c>
       <c r="M52" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.3">
@@ -2740,23 +2743,23 @@
         <v>20210226</v>
       </c>
       <c r="E53" t="str">
-        <f t="shared" si="1"/>
-        <v>JC-SW-GHG-R1-20210226</v>
+        <f>_xlfn.CONCAT(A53,"-",B53,"-",C53,"-",D53)</f>
+        <v>JC-UW1-GHG-R1-20210226</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="I53" s="3">
-        <v>5.4</v>
+        <v>7.3</v>
       </c>
       <c r="J53" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L53">
         <v>0</v>
       </c>
       <c r="M53" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.3">
@@ -2767,29 +2770,29 @@
         <v>1</v>
       </c>
       <c r="C54" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D54">
         <v>20210226</v>
       </c>
       <c r="E54" t="str">
-        <f t="shared" si="1"/>
-        <v>JC-SW-GHG-R2-20210226</v>
+        <f>_xlfn.CONCAT(A54,"-",B54,"-",C54,"-",D54)</f>
+        <v>JC-UW1-GHG-R2-20210226</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="I54" s="3">
-        <v>5.4</v>
+        <v>7.3</v>
       </c>
       <c r="J54" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L54">
         <v>0</v>
       </c>
       <c r="M54" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.3">
@@ -2800,63 +2803,34 @@
         <v>1</v>
       </c>
       <c r="C55" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D55">
         <v>20210226</v>
       </c>
       <c r="E55" t="str">
-        <f t="shared" si="1"/>
-        <v>JC-SW-GHG-R3-20210226</v>
+        <f>_xlfn.CONCAT(A55,"-",B55,"-",C55,"-",D55)</f>
+        <v>JC-UW1-GHG-R3-20210226</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="I55" s="3">
-        <v>5.4</v>
+        <v>7.3</v>
       </c>
       <c r="J55" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L55">
         <v>0</v>
       </c>
       <c r="M55" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A56" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B56" t="s">
-        <v>1</v>
-      </c>
-      <c r="C56" t="s">
-        <v>2</v>
-      </c>
-      <c r="D56">
-        <v>20210226</v>
-      </c>
-      <c r="E56" t="str">
-        <f t="shared" si="1"/>
-        <v>JC-UW1-GHG-R1-20210226</v>
-      </c>
-      <c r="F56" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="I56" s="3">
-        <v>7.3</v>
-      </c>
-      <c r="J56" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="L56">
-        <v>0</v>
-      </c>
-      <c r="M56" t="s">
-        <v>61</v>
-      </c>
+      <c r="A56" s="1"/>
+      <c r="F56" s="6"/>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
@@ -2866,29 +2840,29 @@
         <v>1</v>
       </c>
       <c r="C57" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="D57">
         <v>20210226</v>
       </c>
       <c r="E57" t="str">
-        <f t="shared" si="1"/>
-        <v>JC-UW1-GHG-R2-20210226</v>
+        <f>_xlfn.CONCAT(A57,"-",B57,"-",C57,"-",D57)</f>
+        <v>NB-SW-GHG-R1-20210226</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="I57" s="3">
-        <v>7.3</v>
+        <v>5.2</v>
       </c>
       <c r="J57" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L57">
         <v>0</v>
       </c>
       <c r="M57" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.3">
@@ -2899,62 +2873,62 @@
         <v>1</v>
       </c>
       <c r="C58" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D58">
         <v>20210226</v>
       </c>
       <c r="E58" t="str">
-        <f t="shared" si="1"/>
-        <v>JC-UW1-GHG-R3-20210226</v>
+        <f>_xlfn.CONCAT(A58,"-",B58,"-",C58,"-",D58)</f>
+        <v>NB-SW-GHG-R2-20210226</v>
       </c>
       <c r="F58" s="6" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="I58" s="3">
-        <v>7.3</v>
+        <v>5.2</v>
       </c>
       <c r="J58" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L58">
         <v>0</v>
       </c>
       <c r="M58" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B59" t="s">
         <v>1</v>
       </c>
       <c r="C59" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="D59">
         <v>20210226</v>
       </c>
       <c r="E59" t="str">
-        <f t="shared" si="1"/>
-        <v>NB-SW-GHG-R1-20210226</v>
+        <f>_xlfn.CONCAT(A59,"-",B59,"-",C59,"-",D59)</f>
+        <v>NB-SW-GHG-R3-20210226</v>
       </c>
       <c r="F59" s="6" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="I59" s="3">
         <v>5.2</v>
       </c>
       <c r="J59" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L59">
         <v>0</v>
       </c>
       <c r="M59" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.3">
@@ -2965,29 +2939,29 @@
         <v>1</v>
       </c>
       <c r="C60" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="D60">
-        <v>20210226</v>
+        <v>20210224</v>
       </c>
       <c r="E60" t="str">
-        <f t="shared" si="1"/>
-        <v>NB-SW-GHG-R2-20210226</v>
+        <f>_xlfn.CONCAT(A60,"-",B60,"-",C60,"-",D60)</f>
+        <v>ND-SW-GHG-R1-20210224</v>
       </c>
       <c r="F60" s="6" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="I60" s="3">
-        <v>5.2</v>
+        <v>5.7</v>
       </c>
       <c r="J60" s="3" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="L60">
         <v>0</v>
       </c>
       <c r="M60" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.3">
@@ -2998,62 +2972,62 @@
         <v>1</v>
       </c>
       <c r="C61" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D61">
-        <v>20210226</v>
+        <v>20210224</v>
       </c>
       <c r="E61" t="str">
-        <f t="shared" si="1"/>
-        <v>NB-SW-GHG-R3-20210226</v>
+        <f>_xlfn.CONCAT(A61,"-",B61,"-",C61,"-",D61)</f>
+        <v>ND-SW-GHG-R2-20210224</v>
       </c>
       <c r="F61" s="6" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="I61" s="3">
-        <v>5.2</v>
+        <v>5.7</v>
       </c>
       <c r="J61" s="3" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="L61">
         <v>0</v>
       </c>
       <c r="M61" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B62" t="s">
         <v>1</v>
       </c>
       <c r="C62" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="D62">
         <v>20210224</v>
       </c>
       <c r="E62" t="str">
-        <f t="shared" si="1"/>
-        <v>ND-SW-GHG-R1-20210224</v>
+        <f>_xlfn.CONCAT(A62,"-",B62,"-",C62,"-",D62)</f>
+        <v>ND-SW-GHG-R3-20210224</v>
       </c>
       <c r="F62" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="I62" s="3">
         <v>5.7</v>
       </c>
       <c r="J62" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L62">
         <v>0</v>
       </c>
       <c r="M62" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.3">
@@ -3064,29 +3038,29 @@
         <v>1</v>
       </c>
       <c r="C63" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="D63">
         <v>20210224</v>
       </c>
       <c r="E63" t="str">
-        <f t="shared" si="1"/>
-        <v>ND-SW-GHG-R2-20210224</v>
+        <f>_xlfn.CONCAT(A63,"-",B63,"-",C63,"-",D63)</f>
+        <v>ND-UW1-GHG-R1-20210224</v>
       </c>
       <c r="F63" s="6" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="I63" s="3">
-        <v>5.7</v>
+        <v>8.5</v>
       </c>
       <c r="J63" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L63">
         <v>0</v>
       </c>
       <c r="M63" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.3">
@@ -3097,62 +3071,62 @@
         <v>1</v>
       </c>
       <c r="C64" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D64">
         <v>20210224</v>
       </c>
       <c r="E64" t="str">
-        <f t="shared" si="1"/>
-        <v>ND-SW-GHG-R3-20210224</v>
+        <f>_xlfn.CONCAT(A64,"-",B64,"-",C64,"-",D64)</f>
+        <v>ND-UW1-GHG-R2-20210224</v>
       </c>
       <c r="F64" s="6" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="I64" s="3">
-        <v>5.7</v>
+        <v>8.5</v>
       </c>
       <c r="J64" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L64">
         <v>0</v>
       </c>
       <c r="M64" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B65" t="s">
         <v>1</v>
       </c>
       <c r="C65" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="D65">
         <v>20210224</v>
       </c>
       <c r="E65" t="str">
-        <f t="shared" si="1"/>
-        <v>ND-UW1-GHG-R1-20210224</v>
+        <f>_xlfn.CONCAT(A65,"-",B65,"-",C65,"-",D65)</f>
+        <v>ND-UW1-GHG-R3-20210224</v>
       </c>
       <c r="F65" s="6" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="I65" s="3">
         <v>8.5</v>
       </c>
       <c r="J65" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L65">
         <v>0</v>
       </c>
       <c r="M65" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.3">
@@ -3163,29 +3137,29 @@
         <v>1</v>
       </c>
       <c r="C66" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="D66">
         <v>20210224</v>
       </c>
       <c r="E66" t="str">
-        <f t="shared" ref="E66:E97" si="2">_xlfn.CONCAT(A66,"-",B66,"-",C66,"-",D66)</f>
-        <v>ND-UW1-GHG-R2-20210224</v>
+        <f>_xlfn.CONCAT(A66,"-",B66,"-",C66,"-",D66)</f>
+        <v>ND-UW2-GHG-R1-20210224</v>
       </c>
       <c r="F66" s="6" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="I66" s="3">
-        <v>8.5</v>
+        <v>8.9</v>
       </c>
       <c r="J66" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L66">
         <v>0</v>
       </c>
       <c r="M66" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.3">
@@ -3196,260 +3170,260 @@
         <v>1</v>
       </c>
       <c r="C67" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D67">
         <v>20210224</v>
       </c>
       <c r="E67" t="str">
-        <f t="shared" si="2"/>
-        <v>ND-UW1-GHG-R3-20210224</v>
+        <f>_xlfn.CONCAT(A67,"-",B67,"-",C67,"-",D67)</f>
+        <v>ND-UW2-GHG-R2-20210224</v>
       </c>
       <c r="F67" s="6" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="I67" s="3">
-        <v>8.5</v>
+        <v>8.9</v>
       </c>
       <c r="J67" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L67">
         <v>0</v>
       </c>
       <c r="M67" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B68" t="s">
         <v>1</v>
       </c>
       <c r="C68" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="D68">
         <v>20210224</v>
       </c>
       <c r="E68" t="str">
-        <f t="shared" si="2"/>
-        <v>ND-UW2-GHG-R1-20210224</v>
+        <f>_xlfn.CONCAT(A68,"-",B68,"-",C68,"-",D68)</f>
+        <v>ND-UW2-GHG-R3-20210224</v>
       </c>
       <c r="F68" s="6" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="I68" s="3">
         <v>8.9</v>
       </c>
       <c r="J68" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L68">
         <v>0</v>
       </c>
       <c r="M68" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="B69" t="s">
         <v>1</v>
       </c>
       <c r="C69" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="D69">
         <v>20210224</v>
       </c>
       <c r="E69" t="str">
-        <f t="shared" si="2"/>
-        <v>ND-UW2-GHG-R2-20210224</v>
+        <f>_xlfn.CONCAT(A69,"-",B69,"-",C69,"-",D69)</f>
+        <v>ND-UW3-GHG-R1-20210224</v>
       </c>
       <c r="F69" s="6" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="I69" s="3">
-        <v>8.9</v>
+        <v>7.6</v>
       </c>
       <c r="J69" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L69">
         <v>0</v>
       </c>
       <c r="M69" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="B70" t="s">
         <v>1</v>
       </c>
       <c r="C70" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D70">
         <v>20210224</v>
       </c>
       <c r="E70" t="str">
-        <f t="shared" si="2"/>
-        <v>ND-UW2-GHG-R3-20210224</v>
+        <f>_xlfn.CONCAT(A70,"-",B70,"-",C70,"-",D70)</f>
+        <v>ND-UW3-GHG-R2-20210224</v>
       </c>
       <c r="F70" s="6" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="I70" s="3">
-        <v>8.9</v>
+        <v>7.6</v>
       </c>
       <c r="J70" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L70">
         <v>0</v>
       </c>
       <c r="M70" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B71" t="s">
         <v>1</v>
       </c>
       <c r="C71" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="D71">
         <v>20210224</v>
       </c>
       <c r="E71" t="str">
-        <f t="shared" si="2"/>
-        <v>ND-UW3-GHG-R1-20210224</v>
+        <f>_xlfn.CONCAT(A71,"-",B71,"-",C71,"-",D71)</f>
+        <v>ND-UW3-GHG-R3-20210224</v>
       </c>
       <c r="F71" s="6" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="I71" s="3">
         <v>7.6</v>
       </c>
       <c r="J71" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L71">
         <v>0</v>
       </c>
       <c r="M71" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="B72" t="s">
         <v>1</v>
       </c>
       <c r="C72" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="D72">
-        <v>20210224</v>
+        <v>20210226</v>
       </c>
       <c r="E72" t="str">
-        <f t="shared" si="2"/>
-        <v>ND-UW3-GHG-R2-20210224</v>
+        <f>_xlfn.CONCAT(A72,"-",B72,"-",C72,"-",D72)</f>
+        <v>QB-SW-GHG-R1-20210226</v>
       </c>
       <c r="F72" s="6" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="I72" s="3">
-        <v>7.6</v>
+        <v>6.8</v>
       </c>
       <c r="J72" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="L72">
         <v>0</v>
       </c>
       <c r="M72" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="B73" t="s">
         <v>1</v>
       </c>
       <c r="C73" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D73">
-        <v>20210224</v>
+        <v>20210226</v>
       </c>
       <c r="E73" t="str">
-        <f t="shared" si="2"/>
-        <v>ND-UW3-GHG-R3-20210224</v>
+        <f>_xlfn.CONCAT(A73,"-",B73,"-",C73,"-",D73)</f>
+        <v>QB-SW-GHG-R2-20210226</v>
       </c>
       <c r="F73" s="6" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I73" s="3">
-        <v>7.6</v>
+        <v>6.8</v>
       </c>
       <c r="J73" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="L73">
         <v>0</v>
       </c>
       <c r="M73" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B74" t="s">
         <v>1</v>
       </c>
       <c r="C74" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="D74">
         <v>20210226</v>
       </c>
       <c r="E74" t="str">
-        <f t="shared" si="2"/>
-        <v>QB-SW-GHG-R1-20210226</v>
+        <f>_xlfn.CONCAT(A74,"-",B74,"-",C74,"-",D74)</f>
+        <v>QB-SW-GHG-R3-20210226</v>
       </c>
       <c r="F74" s="6" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I74" s="3">
         <v>6.8</v>
       </c>
       <c r="J74" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L74">
         <v>0</v>
       </c>
       <c r="M74" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.3">
@@ -3460,29 +3434,29 @@
         <v>1</v>
       </c>
       <c r="C75" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="D75">
         <v>20210226</v>
       </c>
       <c r="E75" t="str">
-        <f t="shared" si="2"/>
-        <v>QB-SW-GHG-R2-20210226</v>
+        <f>_xlfn.CONCAT(A75,"-",B75,"-",C75,"-",D75)</f>
+        <v>QB-UW1-GHG-R1-20210226</v>
       </c>
       <c r="F75" s="6" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="I75" s="3">
-        <v>6.8</v>
+        <v>8.6</v>
       </c>
       <c r="J75" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L75">
         <v>0</v>
       </c>
       <c r="M75" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.3">
@@ -3493,62 +3467,62 @@
         <v>1</v>
       </c>
       <c r="C76" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D76">
         <v>20210226</v>
       </c>
       <c r="E76" t="str">
-        <f t="shared" si="2"/>
-        <v>QB-SW-GHG-R3-20210226</v>
+        <f>_xlfn.CONCAT(A76,"-",B76,"-",C76,"-",D76)</f>
+        <v>QB-UW1-GHG-R2-20210226</v>
       </c>
       <c r="F76" s="6" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="I76" s="3">
-        <v>6.8</v>
+        <v>8.6</v>
       </c>
       <c r="J76" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L76">
         <v>0</v>
       </c>
       <c r="M76" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B77" t="s">
         <v>1</v>
       </c>
       <c r="C77" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="D77">
         <v>20210226</v>
       </c>
       <c r="E77" t="str">
-        <f t="shared" si="2"/>
-        <v>QB-UW1-GHG-R1-20210226</v>
+        <f>_xlfn.CONCAT(A77,"-",B77,"-",C77,"-",D77)</f>
+        <v>QB-UW1-GHG-R3-20210226</v>
       </c>
       <c r="F77" s="6" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="I77" s="3">
         <v>8.6</v>
       </c>
       <c r="J77" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L77">
         <v>0</v>
       </c>
       <c r="M77" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.3">
@@ -3559,29 +3533,29 @@
         <v>1</v>
       </c>
       <c r="C78" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="D78">
         <v>20210226</v>
       </c>
       <c r="E78" t="str">
-        <f t="shared" si="2"/>
-        <v>QB-UW1-GHG-R2-20210226</v>
+        <f>_xlfn.CONCAT(A78,"-",B78,"-",C78,"-",D78)</f>
+        <v>QB-UW2-GHG-R1-20210226</v>
       </c>
       <c r="F78" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="I78" s="3">
-        <v>8.6</v>
+        <v>10.4</v>
       </c>
       <c r="J78" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L78">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M78" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.3">
@@ -3592,62 +3566,62 @@
         <v>1</v>
       </c>
       <c r="C79" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D79">
         <v>20210226</v>
       </c>
       <c r="E79" t="str">
-        <f t="shared" si="2"/>
-        <v>QB-UW1-GHG-R3-20210226</v>
+        <f>_xlfn.CONCAT(A79,"-",B79,"-",C79,"-",D79)</f>
+        <v>QB-UW2-GHG-R2-20210226</v>
       </c>
       <c r="F79" s="6" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="I79" s="3">
-        <v>8.6</v>
+        <v>10.4</v>
       </c>
       <c r="J79" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L79">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M79" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B80" t="s">
         <v>1</v>
       </c>
       <c r="C80" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="D80">
         <v>20210226</v>
       </c>
       <c r="E80" t="str">
-        <f t="shared" si="2"/>
-        <v>QB-UW2-GHG-R1-20210226</v>
+        <f>_xlfn.CONCAT(A80,"-",B80,"-",C80,"-",D80)</f>
+        <v>QB-UW2-GHG-R3-20210226</v>
       </c>
       <c r="F80" s="6" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="I80" s="3">
         <v>10.4</v>
       </c>
       <c r="J80" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L80">
         <v>1</v>
       </c>
       <c r="M80" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.3">
@@ -3658,29 +3632,29 @@
         <v>1</v>
       </c>
       <c r="C81" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="D81">
-        <v>20210226</v>
+        <v>20210225</v>
       </c>
       <c r="E81" t="str">
-        <f t="shared" si="2"/>
-        <v>QB-UW2-GHG-R2-20210226</v>
+        <f>_xlfn.CONCAT(A81,"-",B81,"-",C81,"-",D81)</f>
+        <v>TA-SW-GHG-R1-20210225</v>
       </c>
       <c r="F81" s="6" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="I81" s="3">
-        <v>10.4</v>
+        <v>5.2</v>
       </c>
       <c r="J81" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="L81">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M81" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.3">
@@ -3691,62 +3665,62 @@
         <v>1</v>
       </c>
       <c r="C82" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D82">
-        <v>20210226</v>
+        <v>20210225</v>
       </c>
       <c r="E82" t="str">
-        <f t="shared" si="2"/>
-        <v>QB-UW2-GHG-R3-20210226</v>
+        <f>_xlfn.CONCAT(A82,"-",B82,"-",C82,"-",D82)</f>
+        <v>TA-SW-GHG-R2-20210225</v>
       </c>
       <c r="F82" s="6" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="I82" s="3">
-        <v>10.4</v>
+        <v>5.2</v>
       </c>
       <c r="J82" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="L82">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M82" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B83" t="s">
         <v>1</v>
       </c>
       <c r="C83" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="D83">
         <v>20210225</v>
       </c>
       <c r="E83" t="str">
-        <f t="shared" si="2"/>
-        <v>TA-SW-GHG-R1-20210225</v>
+        <f>_xlfn.CONCAT(A83,"-",B83,"-",C83,"-",D83)</f>
+        <v>TA-SW-GHG-R3-20210225</v>
       </c>
       <c r="F83" s="6" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I83" s="3">
         <v>5.2</v>
       </c>
       <c r="J83" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L83">
         <v>0</v>
       </c>
       <c r="M83" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.3">
@@ -3757,29 +3731,29 @@
         <v>1</v>
       </c>
       <c r="C84" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="D84">
         <v>20210225</v>
       </c>
       <c r="E84" t="str">
-        <f t="shared" si="2"/>
-        <v>TA-SW-GHG-R2-20210225</v>
+        <f>_xlfn.CONCAT(A84,"-",B84,"-",C84,"-",D84)</f>
+        <v>TB-SW-GHG-R1-20210225</v>
       </c>
       <c r="F84" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="I84" s="3">
-        <v>5.2</v>
+        <v>6.3</v>
       </c>
       <c r="J84" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L84">
         <v>0</v>
       </c>
       <c r="M84" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.3">
@@ -3790,62 +3764,62 @@
         <v>1</v>
       </c>
       <c r="C85" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D85">
         <v>20210225</v>
       </c>
       <c r="E85" t="str">
-        <f t="shared" si="2"/>
-        <v>TA-SW-GHG-R3-20210225</v>
+        <f>_xlfn.CONCAT(A85,"-",B85,"-",C85,"-",D85)</f>
+        <v>TB-SW-GHG-R2-20210225</v>
       </c>
       <c r="F85" s="6" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="I85" s="3">
-        <v>5.2</v>
+        <v>6.3</v>
       </c>
       <c r="J85" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L85">
         <v>0</v>
       </c>
       <c r="M85" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B86" t="s">
         <v>1</v>
       </c>
       <c r="C86" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="D86">
         <v>20210225</v>
       </c>
       <c r="E86" t="str">
-        <f t="shared" si="2"/>
-        <v>TB-SW-GHG-R1-20210225</v>
+        <f>_xlfn.CONCAT(A86,"-",B86,"-",C86,"-",D86)</f>
+        <v>TB-SW-GHG-R3-20210225</v>
       </c>
       <c r="F86" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="I86" s="3">
         <v>6.3</v>
       </c>
       <c r="J86" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L86">
         <v>0</v>
       </c>
       <c r="M86" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.3">
@@ -3856,29 +3830,29 @@
         <v>1</v>
       </c>
       <c r="C87" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="D87">
         <v>20210225</v>
       </c>
       <c r="E87" t="str">
-        <f t="shared" si="2"/>
-        <v>TB-SW-GHG-R2-20210225</v>
+        <f>_xlfn.CONCAT(A87,"-",B87,"-",C87,"-",D87)</f>
+        <v>TB-UW1-GHG-R1-20210225</v>
       </c>
       <c r="F87" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="I87" s="3">
-        <v>6.3</v>
+        <v>7.7</v>
       </c>
       <c r="J87" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L87">
         <v>0</v>
       </c>
       <c r="M87" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.3">
@@ -3889,62 +3863,62 @@
         <v>1</v>
       </c>
       <c r="C88" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D88">
         <v>20210225</v>
       </c>
       <c r="E88" t="str">
-        <f t="shared" si="2"/>
-        <v>TB-SW-GHG-R3-20210225</v>
+        <f>_xlfn.CONCAT(A88,"-",B88,"-",C88,"-",D88)</f>
+        <v>TB-UW1-GHG-R2-20210225</v>
       </c>
       <c r="F88" s="6" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="I88" s="3">
-        <v>6.3</v>
+        <v>7.7</v>
       </c>
       <c r="J88" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L88">
         <v>0</v>
       </c>
       <c r="M88" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B89" t="s">
         <v>1</v>
       </c>
       <c r="C89" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="D89">
         <v>20210225</v>
       </c>
       <c r="E89" t="str">
-        <f t="shared" si="2"/>
-        <v>TB-UW1-GHG-R1-20210225</v>
+        <f>_xlfn.CONCAT(A89,"-",B89,"-",C89,"-",D89)</f>
+        <v>TB-UW1-GHG-R3-20210225</v>
       </c>
       <c r="F89" s="6" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="I89" s="3">
         <v>7.7</v>
       </c>
       <c r="J89" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L89">
         <v>0</v>
       </c>
       <c r="M89" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.3">
@@ -3955,29 +3929,29 @@
         <v>1</v>
       </c>
       <c r="C90" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="D90">
         <v>20210225</v>
       </c>
       <c r="E90" t="str">
-        <f t="shared" si="2"/>
-        <v>TB-UW1-GHG-R2-20210225</v>
+        <f>_xlfn.CONCAT(A90,"-",B90,"-",C90,"-",D90)</f>
+        <v>TB-UW2-GHG-R1-20210225</v>
       </c>
       <c r="F90" s="6" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="I90" s="3">
-        <v>7.7</v>
+        <v>6.7</v>
       </c>
       <c r="J90" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L90">
         <v>0</v>
       </c>
       <c r="M90" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.3">
@@ -3988,62 +3962,62 @@
         <v>1</v>
       </c>
       <c r="C91" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D91">
         <v>20210225</v>
       </c>
       <c r="E91" t="str">
-        <f t="shared" si="2"/>
-        <v>TB-UW1-GHG-R3-20210225</v>
+        <f>_xlfn.CONCAT(A91,"-",B91,"-",C91,"-",D91)</f>
+        <v>TB-UW2-GHG-R2-20210225</v>
       </c>
       <c r="F91" s="6" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="I91" s="3">
-        <v>7.7</v>
+        <v>6.7</v>
       </c>
       <c r="J91" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L91">
         <v>0</v>
       </c>
       <c r="M91" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B92" t="s">
         <v>1</v>
       </c>
       <c r="C92" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="D92">
         <v>20210225</v>
       </c>
       <c r="E92" t="str">
-        <f t="shared" si="2"/>
-        <v>TB-UW2-GHG-R1-20210225</v>
+        <f>_xlfn.CONCAT(A92,"-",B92,"-",C92,"-",D92)</f>
+        <v>TB-UW2-GHG-R3-20210225</v>
       </c>
       <c r="F92" s="6" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="I92" s="3">
         <v>6.7</v>
       </c>
       <c r="J92" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L92">
         <v>0</v>
       </c>
       <c r="M92" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.3">
@@ -4054,29 +4028,29 @@
         <v>1</v>
       </c>
       <c r="C93" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="D93">
         <v>20210225</v>
       </c>
       <c r="E93" t="str">
-        <f t="shared" si="2"/>
-        <v>TB-UW2-GHG-R2-20210225</v>
+        <f>_xlfn.CONCAT(A93,"-",B93,"-",C93,"-",D93)</f>
+        <v>TB-UW3-GHG-R1-20210225</v>
       </c>
       <c r="F93" s="6" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="I93" s="3">
-        <v>6.7</v>
+        <v>9.5</v>
       </c>
       <c r="J93" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L93">
         <v>0</v>
       </c>
       <c r="M93" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.3">
@@ -4087,62 +4061,62 @@
         <v>1</v>
       </c>
       <c r="C94" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D94">
         <v>20210225</v>
       </c>
       <c r="E94" t="str">
-        <f t="shared" si="2"/>
-        <v>TB-UW2-GHG-R3-20210225</v>
+        <f>_xlfn.CONCAT(A94,"-",B94,"-",C94,"-",D94)</f>
+        <v>TB-UW3-GHG-R2-20210225</v>
       </c>
       <c r="F94" s="6" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="I94" s="3">
-        <v>6.7</v>
+        <v>9.5</v>
       </c>
       <c r="J94" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L94">
         <v>0</v>
       </c>
       <c r="M94" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B95" t="s">
         <v>1</v>
       </c>
       <c r="C95" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="D95">
         <v>20210225</v>
       </c>
       <c r="E95" t="str">
-        <f t="shared" si="2"/>
-        <v>TB-UW3-GHG-R1-20210225</v>
+        <f>_xlfn.CONCAT(A95,"-",B95,"-",C95,"-",D95)</f>
+        <v>TB-UW3-GHG-R3-20210225</v>
       </c>
       <c r="F95" s="6" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="I95" s="3">
         <v>9.5</v>
       </c>
       <c r="J95" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L95">
         <v>0</v>
       </c>
       <c r="M95" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.3">
@@ -4153,20 +4127,20 @@
         <v>1</v>
       </c>
       <c r="C96" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="D96">
-        <v>20210225</v>
+        <v>20210226</v>
       </c>
       <c r="E96" t="str">
-        <f t="shared" si="2"/>
-        <v>TB-UW3-GHG-R2-20210225</v>
+        <f>_xlfn.CONCAT(A96,"-",B96,"-",C96,"-",D96)</f>
+        <v>TI-SW-GHG-R1-20210226</v>
       </c>
       <c r="F96" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="I96" s="3">
-        <v>9.5</v>
+        <v>6.8</v>
       </c>
       <c r="J96" s="3" t="s">
         <v>59</v>
@@ -4175,7 +4149,7 @@
         <v>0</v>
       </c>
       <c r="M96" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.3">
@@ -4186,20 +4160,20 @@
         <v>1</v>
       </c>
       <c r="C97" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D97">
-        <v>20210225</v>
+        <v>20210226</v>
       </c>
       <c r="E97" t="str">
-        <f t="shared" si="2"/>
-        <v>TB-UW3-GHG-R3-20210225</v>
+        <f>_xlfn.CONCAT(A97,"-",B97,"-",C97,"-",D97)</f>
+        <v>TI-SW-GHG-R2-20210226</v>
       </c>
       <c r="F97" s="6" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="I97" s="3">
-        <v>9.5</v>
+        <v>6.8</v>
       </c>
       <c r="J97" s="3" t="s">
         <v>59</v>
@@ -4208,40 +4182,40 @@
         <v>0</v>
       </c>
       <c r="M97" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B98" t="s">
         <v>1</v>
       </c>
       <c r="C98" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="D98">
         <v>20210226</v>
       </c>
       <c r="E98" t="str">
-        <f t="shared" ref="E98:E129" si="3">_xlfn.CONCAT(A98,"-",B98,"-",C98,"-",D98)</f>
-        <v>TI-SW-GHG-R1-20210226</v>
+        <f>_xlfn.CONCAT(A98,"-",B98,"-",C98,"-",D98)</f>
+        <v>TI-SW-GHG-R3-20210226</v>
       </c>
       <c r="F98" s="6" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="I98" s="3">
         <v>6.8</v>
       </c>
       <c r="J98" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L98">
         <v>0</v>
       </c>
       <c r="M98" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.3">
@@ -4252,29 +4226,29 @@
         <v>1</v>
       </c>
       <c r="C99" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="D99">
-        <v>20210226</v>
+        <v>20210225</v>
       </c>
       <c r="E99" t="str">
-        <f t="shared" si="3"/>
-        <v>TI-SW-GHG-R2-20210226</v>
+        <f>_xlfn.CONCAT(A99,"-",B99,"-",C99,"-",D99)</f>
+        <v>TR-SW-GHG-R1-20210225</v>
       </c>
       <c r="F99" s="6" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="I99" s="3">
-        <v>6.8</v>
+        <v>9.5</v>
       </c>
       <c r="J99" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="L99">
         <v>0</v>
       </c>
       <c r="M99" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.3">
@@ -4285,62 +4259,62 @@
         <v>1</v>
       </c>
       <c r="C100" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D100">
-        <v>20210226</v>
+        <v>20210225</v>
       </c>
       <c r="E100" t="str">
-        <f t="shared" si="3"/>
-        <v>TI-SW-GHG-R3-20210226</v>
+        <f>_xlfn.CONCAT(A100,"-",B100,"-",C100,"-",D100)</f>
+        <v>TR-SW-GHG-R2-20210225</v>
       </c>
       <c r="F100" s="6" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="I100" s="3">
-        <v>6.8</v>
+        <v>9.5</v>
       </c>
       <c r="J100" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="L100">
         <v>0</v>
       </c>
       <c r="M100" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B101" t="s">
         <v>1</v>
       </c>
       <c r="C101" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="D101">
         <v>20210225</v>
       </c>
       <c r="E101" t="str">
-        <f t="shared" si="3"/>
-        <v>TR-SW-GHG-R1-20210225</v>
+        <f>_xlfn.CONCAT(A101,"-",B101,"-",C101,"-",D101)</f>
+        <v>TR-SW-GHG-R3-20210225</v>
       </c>
       <c r="F101" s="6" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="I101" s="3">
         <v>9.5</v>
       </c>
       <c r="J101" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L101">
         <v>0</v>
       </c>
       <c r="M101" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.3">
@@ -4351,29 +4325,29 @@
         <v>1</v>
       </c>
       <c r="C102" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="D102">
-        <v>20210225</v>
+        <v>20210224</v>
       </c>
       <c r="E102" t="str">
-        <f t="shared" si="3"/>
-        <v>TR-SW-GHG-R2-20210225</v>
+        <f>_xlfn.CONCAT(A102,"-",B102,"-",C102,"-",D102)</f>
+        <v>TS-SW-GHG-R1-20210224</v>
       </c>
       <c r="F102" s="6" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="I102" s="3">
-        <v>9.5</v>
+        <v>4.2</v>
       </c>
       <c r="J102" s="3" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="L102">
         <v>0</v>
       </c>
       <c r="M102" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.3">
@@ -4384,327 +4358,267 @@
         <v>1</v>
       </c>
       <c r="C103" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D103">
-        <v>20210225</v>
+        <v>20210224</v>
       </c>
       <c r="E103" t="str">
-        <f t="shared" si="3"/>
-        <v>TR-SW-GHG-R3-20210225</v>
+        <f>_xlfn.CONCAT(A103,"-",B103,"-",C103,"-",D103)</f>
+        <v>TS-SW-GHG-R2-20210224</v>
       </c>
       <c r="F103" s="6" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="I103" s="3">
-        <v>9.5</v>
+        <v>4.2</v>
       </c>
       <c r="J103" s="3" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="L103">
         <v>0</v>
       </c>
       <c r="M103" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
-        <v>67</v>
+        <v>32</v>
       </c>
       <c r="B104" t="s">
         <v>1</v>
       </c>
       <c r="C104" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="D104">
         <v>20210224</v>
       </c>
       <c r="E104" t="str">
-        <f t="shared" si="3"/>
-        <v>TS-CH-GHG-R1-20210224</v>
+        <f>_xlfn.CONCAT(A104,"-",B104,"-",C104,"-",D104)</f>
+        <v>TS-SW-GHG-R3-20210224</v>
       </c>
       <c r="F104" s="6" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="I104" s="3">
-        <v>8.6</v>
+        <v>4.2</v>
       </c>
       <c r="J104" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L104">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M104" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B105" t="s">
         <v>1</v>
       </c>
       <c r="C105" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="D105">
         <v>20210224</v>
       </c>
       <c r="E105" t="str">
-        <f t="shared" si="3"/>
-        <v>TS-CH-GHG-R2-20210224</v>
+        <f>_xlfn.CONCAT(A105,"-",B105,"-",C105,"-",D105)</f>
+        <v>TS-CH-GHG-R1-20210224</v>
       </c>
       <c r="F105" s="6" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I105" s="3">
         <v>8.6</v>
       </c>
       <c r="J105" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L105">
         <v>1</v>
       </c>
       <c r="M105" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B106" t="s">
         <v>1</v>
       </c>
       <c r="C106" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D106">
         <v>20210224</v>
       </c>
       <c r="E106" t="str">
-        <f t="shared" si="3"/>
-        <v>TS-CH-GHG-R3-20210224</v>
+        <f>_xlfn.CONCAT(A106,"-",B106,"-",C106,"-",D106)</f>
+        <v>TS-CH-GHG-R2-20210224</v>
       </c>
       <c r="F106" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="I106" s="3">
         <v>8.6</v>
       </c>
       <c r="J106" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L106">
         <v>1</v>
       </c>
       <c r="M106" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="B107" t="s">
         <v>1</v>
       </c>
       <c r="C107" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="D107">
         <v>20210224</v>
       </c>
       <c r="E107" t="str">
-        <f t="shared" si="3"/>
-        <v>TS-SW-GHG-R1-20210224</v>
+        <f>_xlfn.CONCAT(A107,"-",B107,"-",C107,"-",D107)</f>
+        <v>TS-CH-GHG-R3-20210224</v>
       </c>
       <c r="F107" s="6" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="I107" s="3">
-        <v>4.2</v>
+        <v>8.6</v>
       </c>
       <c r="J107" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L107">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M107" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="B108" t="s">
         <v>1</v>
       </c>
       <c r="C108" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="D108">
         <v>20210224</v>
       </c>
       <c r="E108" t="str">
-        <f t="shared" si="3"/>
-        <v>TS-SW-GHG-R2-20210224</v>
+        <f>_xlfn.CONCAT(A108,"-",B108,"-",C108,"-",D108)</f>
+        <v>TS-UW1-GHG-R1-20210224</v>
       </c>
       <c r="F108" s="6" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="I108" s="3">
-        <v>4.2</v>
+        <v>8</v>
       </c>
       <c r="J108" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L108">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M108" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B109" t="s">
+        <v>1</v>
+      </c>
+      <c r="C109" t="s">
         <v>33</v>
-      </c>
-      <c r="B109" t="s">
-        <v>1</v>
-      </c>
-      <c r="C109" t="s">
-        <v>35</v>
       </c>
       <c r="D109">
         <v>20210224</v>
       </c>
       <c r="E109" t="str">
-        <f t="shared" si="3"/>
-        <v>TS-SW-GHG-R3-20210224</v>
+        <f>_xlfn.CONCAT(A109,"-",B109,"-",C109,"-",D109)</f>
+        <v>TS-UW1-GHG-R2-20210224</v>
       </c>
       <c r="F109" s="6" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="I109" s="3">
-        <v>4.2</v>
+        <v>8</v>
       </c>
       <c r="J109" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L109">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M109" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B110" t="s">
         <v>1</v>
       </c>
       <c r="C110" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="D110">
         <v>20210224</v>
       </c>
       <c r="E110" t="str">
-        <f t="shared" si="3"/>
-        <v>TS-UW1-GHG-R1-20210224</v>
+        <f>_xlfn.CONCAT(A110,"-",B110,"-",C110,"-",D110)</f>
+        <v>TS-UW1-GHG-R3-20210224</v>
       </c>
       <c r="F110" s="6" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I110" s="3">
         <v>8</v>
       </c>
       <c r="J110" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L110">
         <v>1</v>
       </c>
       <c r="M110" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A111" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B111" t="s">
-        <v>1</v>
-      </c>
-      <c r="C111" t="s">
-        <v>34</v>
-      </c>
-      <c r="D111">
-        <v>20210224</v>
-      </c>
-      <c r="E111" t="str">
-        <f t="shared" si="3"/>
-        <v>TS-UW1-GHG-R2-20210224</v>
-      </c>
-      <c r="F111" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="I111" s="3">
-        <v>8</v>
-      </c>
-      <c r="J111" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="L111">
-        <v>1</v>
-      </c>
-      <c r="M111" t="s">
-        <v>70</v>
-      </c>
+      <c r="F111" s="6"/>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A112" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B112" t="s">
-        <v>1</v>
-      </c>
-      <c r="C112" t="s">
-        <v>35</v>
-      </c>
-      <c r="D112">
-        <v>20210224</v>
-      </c>
-      <c r="E112" t="str">
-        <f t="shared" si="3"/>
-        <v>TS-UW1-GHG-R3-20210224</v>
-      </c>
-      <c r="F112" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="I112" s="3">
-        <v>8</v>
-      </c>
-      <c r="J112" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="L112">
-        <v>1</v>
-      </c>
-      <c r="M112" t="s">
-        <v>70</v>
-      </c>
+      <c r="F112" s="6"/>
     </row>
     <row r="113" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F113" s="6"/>
@@ -4733,15 +4647,9 @@
     <row r="121" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F121" s="6"/>
     </row>
-    <row r="122" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F122" s="6"/>
-    </row>
-    <row r="123" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F123" s="6"/>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M112">
-    <sortCondition ref="A2:A112"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M121">
+    <sortCondition ref="F2:F121"/>
   </sortState>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4768,28 +4676,28 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" t="s">
         <v>42</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>43</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>44</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>45</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>46</v>
       </c>
-      <c r="G1" t="s">
-        <v>47</v>
-      </c>
       <c r="H1" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I1" s="3"/>
     </row>
@@ -4829,51 +4737,51 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="F9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="H9" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="J9" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I9" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="J9" s="2" t="s">
+      <c r="K9" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="L9" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" t="s">
         <v>71</v>
-      </c>
-      <c r="C10" t="s">
-        <v>72</v>
       </c>
       <c r="D10">
         <v>20210225</v>
@@ -4886,24 +4794,24 @@
         <v>6.3</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K10">
         <v>0</v>
       </c>
       <c r="L10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" t="s">
         <v>71</v>
-      </c>
-      <c r="C11" t="s">
-        <v>72</v>
       </c>
       <c r="D11">
         <v>20210225</v>
@@ -4916,13 +4824,13 @@
         <v>6.7</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K11">
         <v>0</v>
       </c>
       <c r="L11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
@@ -4930,10 +4838,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" t="s">
         <v>71</v>
-      </c>
-      <c r="C12" t="s">
-        <v>72</v>
       </c>
       <c r="D12">
         <v>20210225</v>
@@ -4946,24 +4854,24 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K12">
         <v>0</v>
       </c>
       <c r="L12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" t="s">
         <v>71</v>
-      </c>
-      <c r="C13" t="s">
-        <v>72</v>
       </c>
       <c r="D13">
         <v>20210226</v>
@@ -4976,24 +4884,24 @@
         <v>6.8</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K13">
         <v>0</v>
       </c>
       <c r="L13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" t="s">
         <v>71</v>
-      </c>
-      <c r="C14" t="s">
-        <v>72</v>
       </c>
       <c r="D14">
         <v>20210226</v>
@@ -5006,13 +4914,13 @@
         <v>8.6</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K14">
         <v>0</v>
       </c>
       <c r="L14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
@@ -5020,10 +4928,10 @@
         <v>7</v>
       </c>
       <c r="B15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" t="s">
         <v>71</v>
-      </c>
-      <c r="C15" t="s">
-        <v>72</v>
       </c>
       <c r="D15">
         <v>20210226</v>
@@ -5036,13 +4944,13 @@
         <v>7.9</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K15">
         <v>0</v>
       </c>
       <c r="L15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>